<commit_message>
updated all hw1 files, new slides, new R files, new and cleaned GSS files
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9900" yWindow="0" windowWidth="25600" windowHeight="15420" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="118">
   <si>
     <t>Topic</t>
   </si>
@@ -287,12 +287,6 @@
     <t>Ch. 11; Ch. 14</t>
   </si>
   <si>
-    <t>Introduction to Quantitative Datasets</t>
-  </si>
-  <si>
-    <t>Exploring Quantitative Datasets</t>
-  </si>
-  <si>
     <t>Introduction to Univariate Statistics</t>
   </si>
   <si>
@@ -323,9 +317,6 @@
     <t>Exam 1 (9/21)</t>
   </si>
   <si>
-    <t>Download R and R Studio; Select Variables for Final Project</t>
-  </si>
-  <si>
     <t>Research Design, Variables, and Causality</t>
   </si>
   <si>
@@ -338,12 +329,6 @@
     <t>Review Day for Exam 1</t>
   </si>
   <si>
-    <t>HW 1 (Due 10/14)</t>
-  </si>
-  <si>
-    <t>HW 2 (Due 10/41)</t>
-  </si>
-  <si>
     <t>HW 3 (Due 10/28)</t>
   </si>
   <si>
@@ -384,6 +369,12 @@
   </si>
   <si>
     <t>Draft Data/Methods Section (Due 12/9 @ 5pm)</t>
+  </si>
+  <si>
+    <t>HW 2 (Due 10/21)</t>
+  </si>
+  <si>
+    <t>Download R and R Studio; Select Variables for Final Project; HW 1 (Due 10/14)</t>
   </si>
 </sst>
 </file>
@@ -527,8 +518,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="95">
+  <cellStyleXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -734,14 +731,128 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -749,16 +860,10 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -770,116 +875,8 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="95">
+  <cellStyles count="101">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -927,6 +924,9 @@
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -974,6 +974,9 @@
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1305,8 +1308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22:E23"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B34" sqref="A1:E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0"/>
@@ -1320,441 +1323,435 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="19" customHeight="1">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="72" t="s">
+      <c r="E1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="63"/>
+      <c r="F1" s="39"/>
     </row>
     <row r="2" spans="1:6" ht="19" customHeight="1">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65" t="s">
+      <c r="D2" s="60"/>
+      <c r="E2" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="63"/>
+      <c r="F2" s="39"/>
     </row>
     <row r="3" spans="1:6" ht="24" customHeight="1">
-      <c r="A3" s="64"/>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="63"/>
+      <c r="A3" s="59"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="39"/>
     </row>
     <row r="4" spans="1:6" ht="26">
-      <c r="A4" s="66" t="s">
+      <c r="A4" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="54" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="39"/>
+    </row>
+    <row r="5" spans="1:6" ht="26">
+      <c r="A5" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="39"/>
+    </row>
+    <row r="6" spans="1:6" ht="15">
+      <c r="A6" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="39"/>
+    </row>
+    <row r="7" spans="1:6" ht="26">
+      <c r="A7" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="39"/>
+    </row>
+    <row r="8" spans="1:6" ht="19" customHeight="1">
+      <c r="A8" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="39"/>
+    </row>
+    <row r="9" spans="1:6" ht="19" customHeight="1">
+      <c r="A9" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="43"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="39"/>
+    </row>
+    <row r="10" spans="1:6" ht="19" customHeight="1">
+      <c r="A10" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="57" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="39"/>
+    </row>
+    <row r="11" spans="1:6" ht="19" customHeight="1">
+      <c r="A11" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="56" t="s">
+        <v>97</v>
+      </c>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="39"/>
+    </row>
+    <row r="12" spans="1:6" ht="26" customHeight="1">
+      <c r="A12" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="B12" s="54" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="54" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="39"/>
+    </row>
+    <row r="13" spans="1:6" ht="15">
+      <c r="A13" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="55"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="39"/>
+    </row>
+    <row r="14" spans="1:6" ht="26" customHeight="1">
+      <c r="A14" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" s="57" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="57" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="52"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="39"/>
+    </row>
+    <row r="15" spans="1:6" ht="15">
+      <c r="A15" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="58"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="39"/>
+    </row>
+    <row r="16" spans="1:6" ht="26">
+      <c r="A16" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="F16" s="39"/>
+    </row>
+    <row r="17" spans="1:8" ht="15">
+      <c r="A17" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="39"/>
+    </row>
+    <row r="18" spans="1:8" ht="19" customHeight="1">
+      <c r="A18" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="67" t="s">
+      <c r="B18" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="57" t="s">
+        <v>116</v>
+      </c>
+      <c r="F18" s="39"/>
+    </row>
+    <row r="19" spans="1:8" ht="19" customHeight="1">
+      <c r="A19" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="51" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="39"/>
+    </row>
+    <row r="20" spans="1:8" ht="26">
+      <c r="A20" s="40" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="C4" s="67" t="s">
-        <v>115</v>
-      </c>
-      <c r="D4" s="68" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="68" t="s">
-        <v>81</v>
-      </c>
-      <c r="F4" s="63"/>
-    </row>
-    <row r="5" spans="1:6" ht="26">
-      <c r="A5" s="69" t="s">
-        <v>69</v>
-      </c>
-      <c r="B5" s="70" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5" s="70" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="63"/>
-    </row>
-    <row r="6" spans="1:6" ht="15">
-      <c r="A6" s="66" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="86" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="63"/>
-    </row>
-    <row r="7" spans="1:6" ht="26">
-      <c r="A7" s="69" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="80" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" s="80" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="80"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="63"/>
-    </row>
-    <row r="8" spans="1:6" ht="19" customHeight="1">
-      <c r="A8" s="66" t="s">
-        <v>109</v>
-      </c>
-      <c r="B8" s="67" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" s="67" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" s="74"/>
-      <c r="E8" s="74"/>
-      <c r="F8" s="63"/>
-    </row>
-    <row r="9" spans="1:6" ht="19" customHeight="1">
-      <c r="A9" s="69" t="s">
-        <v>68</v>
-      </c>
-      <c r="B9" s="70" t="s">
-        <v>103</v>
-      </c>
-      <c r="C9" s="70"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="63"/>
-    </row>
-    <row r="10" spans="1:6" ht="19" customHeight="1">
-      <c r="A10" s="66" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="79" t="s">
-        <v>104</v>
-      </c>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="63"/>
-    </row>
-    <row r="11" spans="1:6" ht="19" customHeight="1">
-      <c r="A11" s="69" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" s="81" t="s">
-        <v>99</v>
-      </c>
-      <c r="C11" s="81"/>
-      <c r="D11" s="81"/>
-      <c r="E11" s="81"/>
-      <c r="F11" s="63"/>
-    </row>
-    <row r="12" spans="1:6" ht="26">
-      <c r="A12" s="66" t="s">
-        <v>110</v>
-      </c>
-      <c r="B12" s="67" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" s="67" t="s">
-        <v>116</v>
-      </c>
-      <c r="D12" s="67"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="63"/>
-    </row>
-    <row r="13" spans="1:6" ht="26">
-      <c r="A13" s="69" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" s="70" t="s">
-        <v>86</v>
-      </c>
-      <c r="C13" s="70" t="s">
-        <v>87</v>
-      </c>
-      <c r="D13" s="70"/>
-      <c r="E13" s="70"/>
-      <c r="F13" s="63"/>
-    </row>
-    <row r="14" spans="1:6" ht="26">
-      <c r="A14" s="66" t="s">
-        <v>111</v>
-      </c>
-      <c r="B14" s="82" t="s">
-        <v>88</v>
-      </c>
-      <c r="C14" s="82"/>
-      <c r="D14" s="82"/>
-      <c r="E14" s="79" t="s">
-        <v>100</v>
-      </c>
-      <c r="F14" s="63"/>
-    </row>
-    <row r="15" spans="1:6" ht="15">
-      <c r="A15" s="69" t="s">
-        <v>75</v>
-      </c>
-      <c r="B15" s="80" t="s">
-        <v>89</v>
-      </c>
-      <c r="C15" s="80"/>
-      <c r="D15" s="80"/>
-      <c r="E15" s="83"/>
-      <c r="F15" s="63"/>
-    </row>
-    <row r="16" spans="1:6" ht="26">
-      <c r="A16" s="66" t="s">
-        <v>112</v>
-      </c>
-      <c r="B16" s="67" t="s">
-        <v>90</v>
-      </c>
-      <c r="C16" s="67"/>
-      <c r="D16" s="67"/>
-      <c r="E16" s="68" t="s">
-        <v>105</v>
-      </c>
-      <c r="F16" s="63"/>
-    </row>
-    <row r="17" spans="1:8" ht="15">
-      <c r="A17" s="69" t="s">
-        <v>76</v>
-      </c>
-      <c r="B17" s="70" t="s">
-        <v>91</v>
-      </c>
-      <c r="C17" s="70"/>
-      <c r="D17" s="70"/>
-      <c r="E17" s="71"/>
-      <c r="F17" s="63"/>
-    </row>
-    <row r="18" spans="1:8" ht="19" customHeight="1">
-      <c r="A18" s="66" t="s">
-        <v>113</v>
-      </c>
-      <c r="B18" s="82" t="s">
-        <v>92</v>
-      </c>
-      <c r="C18" s="82"/>
-      <c r="D18" s="82"/>
-      <c r="E18" s="79" t="s">
-        <v>106</v>
-      </c>
-      <c r="F18" s="63"/>
-    </row>
-    <row r="19" spans="1:8" ht="19" customHeight="1">
-      <c r="A19" s="69" t="s">
-        <v>77</v>
-      </c>
-      <c r="B19" s="80" t="s">
+      <c r="F20" s="39"/>
+    </row>
+    <row r="21" spans="1:8" ht="24" customHeight="1">
+      <c r="A21" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="C19" s="80"/>
-      <c r="D19" s="80"/>
-      <c r="E19" s="83"/>
-      <c r="F19" s="63"/>
-    </row>
-    <row r="20" spans="1:8" ht="26">
-      <c r="A20" s="66" t="s">
-        <v>114</v>
-      </c>
-      <c r="B20" s="67" t="s">
-        <v>94</v>
-      </c>
-      <c r="C20" s="76"/>
-      <c r="D20" s="76"/>
-      <c r="E20" s="68" t="s">
-        <v>107</v>
-      </c>
-      <c r="F20" s="63"/>
-    </row>
-    <row r="21" spans="1:8" ht="24" customHeight="1">
-      <c r="A21" s="69" t="s">
-        <v>78</v>
-      </c>
-      <c r="B21" s="70" t="s">
-        <v>95</v>
-      </c>
-      <c r="C21" s="77"/>
-      <c r="D21" s="77"/>
-      <c r="E21" s="71"/>
-      <c r="F21" s="63"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="39"/>
       <c r="H21" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="23" customHeight="1">
-      <c r="A22" s="68" t="s">
+      <c r="A22" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="82" t="s">
-        <v>96</v>
-      </c>
-      <c r="C22" s="82" t="s">
-        <v>97</v>
-      </c>
-      <c r="D22" s="82"/>
-      <c r="E22" s="79" t="s">
-        <v>117</v>
-      </c>
-      <c r="F22" s="63"/>
+      <c r="B22" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="52"/>
+      <c r="E22" s="57" t="s">
+        <v>112</v>
+      </c>
+      <c r="F22" s="39"/>
     </row>
     <row r="23" spans="1:8" ht="20" customHeight="1">
-      <c r="A23" s="71"/>
-      <c r="B23" s="80"/>
-      <c r="C23" s="80"/>
-      <c r="D23" s="80"/>
-      <c r="E23" s="83"/>
-      <c r="F23" s="63"/>
+      <c r="A23" s="55"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="39"/>
       <c r="H23" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="32" customHeight="1">
-      <c r="A24" s="68" t="s">
+      <c r="A24" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="68" t="s">
-        <v>98</v>
-      </c>
-      <c r="C24" s="67"/>
-      <c r="D24" s="68" t="s">
+      <c r="B24" s="54" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" s="41"/>
+      <c r="D24" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="E24" s="68" t="s">
-        <v>118</v>
-      </c>
-      <c r="F24" s="63"/>
+      <c r="E24" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="F24" s="39"/>
     </row>
     <row r="25" spans="1:8" ht="15">
-      <c r="A25" s="71"/>
-      <c r="B25" s="71"/>
-      <c r="C25" s="70"/>
-      <c r="D25" s="71"/>
-      <c r="E25" s="71"/>
-      <c r="F25" s="63"/>
+      <c r="A25" s="55"/>
+      <c r="B25" s="55"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="39"/>
     </row>
     <row r="26" spans="1:8" ht="19" customHeight="1">
-      <c r="A26" s="68" t="s">
+      <c r="A26" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="82" t="s">
+      <c r="B26" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="82"/>
-      <c r="D26" s="82" t="s">
+      <c r="C26" s="52"/>
+      <c r="D26" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="82"/>
-      <c r="F26" s="63"/>
+      <c r="E26" s="52"/>
+      <c r="F26" s="39"/>
     </row>
     <row r="27" spans="1:8" ht="15">
-      <c r="A27" s="71"/>
-      <c r="B27" s="80"/>
-      <c r="C27" s="80"/>
-      <c r="D27" s="80"/>
-      <c r="E27" s="80"/>
-      <c r="F27" s="63"/>
+      <c r="A27" s="55"/>
+      <c r="B27" s="51"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="39"/>
     </row>
     <row r="28" spans="1:8" ht="19" customHeight="1">
-      <c r="A28" s="68" t="s">
+      <c r="A28" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="68" t="s">
+      <c r="B28" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="68"/>
-      <c r="D28" s="68"/>
-      <c r="E28" s="68"/>
-      <c r="F28" s="63"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="39"/>
     </row>
     <row r="29" spans="1:8" ht="19" customHeight="1">
-      <c r="A29" s="71"/>
-      <c r="B29" s="71"/>
-      <c r="C29" s="71"/>
-      <c r="D29" s="71"/>
-      <c r="E29" s="71"/>
-      <c r="F29" s="63"/>
+      <c r="A29" s="55"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="39"/>
     </row>
     <row r="30" spans="1:8" ht="22" customHeight="1">
-      <c r="A30" s="68" t="s">
+      <c r="A30" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="B30" s="79" t="s">
+      <c r="B30" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="79"/>
-      <c r="D30" s="79"/>
-      <c r="E30" s="79" t="s">
-        <v>119</v>
-      </c>
-      <c r="F30" s="63"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F30" s="39"/>
     </row>
     <row r="31" spans="1:8" ht="19" customHeight="1">
-      <c r="A31" s="71"/>
-      <c r="B31" s="83"/>
-      <c r="C31" s="83"/>
-      <c r="D31" s="83"/>
-      <c r="E31" s="83"/>
-      <c r="F31" s="63"/>
+      <c r="A31" s="55"/>
+      <c r="B31" s="58"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="58"/>
+      <c r="F31" s="39"/>
     </row>
     <row r="32" spans="1:8" ht="19" customHeight="1">
-      <c r="A32" s="68" t="s">
+      <c r="A32" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="68" t="s">
+      <c r="B32" s="54" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="67"/>
-      <c r="D32" s="67"/>
-      <c r="E32" s="68" t="s">
-        <v>120</v>
-      </c>
-      <c r="F32" s="63"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="F32" s="39"/>
     </row>
     <row r="33" spans="1:6" ht="19" customHeight="1">
-      <c r="A33" s="71"/>
-      <c r="B33" s="71"/>
-      <c r="C33" s="70"/>
-      <c r="D33" s="70"/>
-      <c r="E33" s="71"/>
-      <c r="F33" s="63"/>
+      <c r="A33" s="55"/>
+      <c r="B33" s="55"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="55"/>
+      <c r="F33" s="39"/>
     </row>
     <row r="34" spans="1:6" ht="19" customHeight="1">
-      <c r="A34" s="78" t="s">
+      <c r="A34" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="84" t="s">
+      <c r="B34" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="84"/>
-      <c r="D34" s="84"/>
-      <c r="E34" s="84"/>
-      <c r="F34" s="63"/>
+      <c r="C34" s="63"/>
+      <c r="D34" s="63"/>
+      <c r="E34" s="63"/>
+      <c r="F34" s="39"/>
     </row>
     <row r="35" spans="1:6" ht="19" customHeight="1">
-      <c r="A35" s="85"/>
+      <c r="A35" s="53"/>
       <c r="B35" s="6"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
@@ -1765,13 +1762,13 @@
       <c r="D36" s="4"/>
     </row>
     <row r="37" spans="1:6" ht="19" customHeight="1">
-      <c r="B37" s="39"/>
-      <c r="C37" s="39"/>
+      <c r="B37" s="61"/>
+      <c r="C37" s="61"/>
       <c r="D37" s="1"/>
     </row>
     <row r="38" spans="1:6" ht="19" customHeight="1">
-      <c r="B38" s="39"/>
-      <c r="C38" s="39"/>
+      <c r="B38" s="61"/>
+      <c r="C38" s="61"/>
       <c r="D38" s="1"/>
     </row>
     <row r="39" spans="1:6" ht="19" customHeight="1">
@@ -1845,7 +1842,29 @@
       <c r="D53" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
+  <mergeCells count="38">
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="B28:E29"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="D4:D5"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A32:A33"/>
     <mergeCell ref="E32:E33"/>
@@ -1862,24 +1881,6 @@
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="B28:E29"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B34:E34"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1928,61 +1929,61 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="19" customHeight="1">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="66" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="21" customHeight="1">
-      <c r="A3" s="59"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="41"/>
+      <c r="A3" s="65"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="67"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="46" t="s">
+      <c r="D4" s="78" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="59"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
       <c r="E5" s="17"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="19" t="s">
@@ -2000,262 +2001,262 @@
       <c r="E7" s="17"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="58" t="s">
+      <c r="A8" s="64" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="66" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="11"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="59"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="41"/>
+      <c r="A9" s="65"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="67"/>
       <c r="E9" s="22"/>
     </row>
     <row r="10" spans="1:5" ht="19" customHeight="1">
-      <c r="A10" s="58" t="s">
+      <c r="A10" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="74" t="s">
         <v>24</v>
       </c>
       <c r="C10" s="23"/>
-      <c r="D10" s="44" t="s">
+      <c r="D10" s="74" t="s">
         <v>41</v>
       </c>
       <c r="E10" s="24"/>
     </row>
     <row r="11" spans="1:5" ht="21" customHeight="1">
-      <c r="A11" s="59"/>
-      <c r="B11" s="45"/>
+      <c r="A11" s="65"/>
+      <c r="B11" s="75"/>
       <c r="C11" s="25"/>
-      <c r="D11" s="45"/>
+      <c r="D11" s="75"/>
       <c r="E11" s="26"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="58" t="s">
+      <c r="A12" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="66" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="27"/>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="66" t="s">
         <v>19</v>
       </c>
       <c r="E12" s="11"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="59"/>
-      <c r="B13" s="41"/>
+      <c r="A13" s="65"/>
+      <c r="B13" s="67"/>
       <c r="C13" s="22"/>
-      <c r="D13" s="41"/>
+      <c r="D13" s="67"/>
       <c r="E13" s="22"/>
     </row>
     <row r="14" spans="1:5" ht="21" customHeight="1">
-      <c r="A14" s="58" t="s">
+      <c r="A14" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="46" t="s">
+      <c r="C14" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="44" t="s">
+      <c r="D14" s="74" t="s">
         <v>20</v>
       </c>
       <c r="E14" s="24"/>
     </row>
     <row r="15" spans="1:5" ht="20" customHeight="1">
-      <c r="A15" s="59"/>
-      <c r="B15" s="45"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="45"/>
+      <c r="A15" s="65"/>
+      <c r="B15" s="75"/>
+      <c r="C15" s="79"/>
+      <c r="D15" s="75"/>
       <c r="E15" s="17"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="60" t="s">
+      <c r="A16" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="48" t="s">
+      <c r="B16" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="49" t="s">
+      <c r="C16" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="48" t="s">
+      <c r="D16" s="84" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="13"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="60"/>
-      <c r="B17" s="48"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="48"/>
+      <c r="A17" s="69"/>
+      <c r="B17" s="84"/>
+      <c r="C17" s="85"/>
+      <c r="D17" s="84"/>
       <c r="E17" s="12"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="60" t="s">
+      <c r="A18" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="52" t="s">
+      <c r="C18" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="51" t="s">
+      <c r="D18" s="82" t="s">
         <v>32</v>
       </c>
       <c r="E18" s="14"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="59"/>
-      <c r="B19" s="45"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="45"/>
+      <c r="A19" s="65"/>
+      <c r="B19" s="75"/>
+      <c r="C19" s="79"/>
+      <c r="D19" s="75"/>
       <c r="E19" s="17"/>
     </row>
     <row r="20" spans="1:5" ht="20" customHeight="1">
-      <c r="A20" s="58" t="s">
+      <c r="A20" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="40" t="s">
+      <c r="D20" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="40" t="s">
+      <c r="E20" s="66" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="19" customHeight="1">
-      <c r="A21" s="59"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
+      <c r="A21" s="65"/>
+      <c r="B21" s="67"/>
+      <c r="C21" s="81"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="67"/>
     </row>
     <row r="22" spans="1:5" ht="21" customHeight="1">
-      <c r="A22" s="58" t="s">
+      <c r="A22" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="55" t="s">
+      <c r="B22" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="46"/>
-      <c r="D22" s="44" t="s">
+      <c r="C22" s="78"/>
+      <c r="D22" s="74" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="44" t="s">
+      <c r="E22" s="74" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="19" customHeight="1">
-      <c r="A23" s="59"/>
-      <c r="B23" s="56"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
+      <c r="A23" s="65"/>
+      <c r="B23" s="77"/>
+      <c r="C23" s="79"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="75"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="58" t="s">
+      <c r="A24" s="64" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="40" t="s">
+      <c r="B24" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42" t="s">
+      <c r="C24" s="80"/>
+      <c r="D24" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="E24" s="40"/>
+      <c r="E24" s="66"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="59"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="41"/>
+      <c r="A25" s="65"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="81"/>
+      <c r="D25" s="81"/>
+      <c r="E25" s="67"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="58" t="s">
+      <c r="A26" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="61" t="s">
+      <c r="B26" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="44" t="s">
+      <c r="C26" s="72"/>
+      <c r="D26" s="72"/>
+      <c r="E26" s="74" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="59"/>
-      <c r="B27" s="62"/>
-      <c r="C27" s="54"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="45"/>
+      <c r="A27" s="65"/>
+      <c r="B27" s="71"/>
+      <c r="C27" s="73"/>
+      <c r="D27" s="73"/>
+      <c r="E27" s="75"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="58" t="s">
+      <c r="A28" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="40"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="40"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="66"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="59"/>
-      <c r="B29" s="41"/>
-      <c r="C29" s="41"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="41"/>
+      <c r="A29" s="65"/>
+      <c r="B29" s="67"/>
+      <c r="C29" s="67"/>
+      <c r="D29" s="67"/>
+      <c r="E29" s="67"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="58" t="s">
+      <c r="A30" s="64" t="s">
         <v>63</v>
       </c>
-      <c r="B30" s="61" t="s">
+      <c r="B30" s="70" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="53"/>
-      <c r="D30" s="53"/>
-      <c r="E30" s="55" t="s">
+      <c r="C30" s="72"/>
+      <c r="D30" s="72"/>
+      <c r="E30" s="76" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="59"/>
-      <c r="B31" s="62"/>
-      <c r="C31" s="54"/>
-      <c r="D31" s="54"/>
-      <c r="E31" s="56"/>
+      <c r="A31" s="65"/>
+      <c r="B31" s="71"/>
+      <c r="C31" s="73"/>
+      <c r="D31" s="73"/>
+      <c r="E31" s="77"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="58" t="s">
+      <c r="A32" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="40" t="s">
+      <c r="B32" s="66" t="s">
         <v>35</v>
       </c>
       <c r="C32" s="11"/>
@@ -2263,8 +2264,8 @@
       <c r="E32" s="28"/>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="59"/>
-      <c r="B33" s="41"/>
+      <c r="A33" s="65"/>
+      <c r="B33" s="67"/>
       <c r="C33" s="29"/>
       <c r="D33" s="29"/>
       <c r="E33" s="30"/>
@@ -2273,22 +2274,54 @@
       <c r="A34" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="57" t="s">
+      <c r="B34" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="57"/>
-      <c r="D34" s="57"/>
-      <c r="E34" s="57"/>
+      <c r="C34" s="68"/>
+      <c r="D34" s="68"/>
+      <c r="E34" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
     <mergeCell ref="B32:B33"/>
     <mergeCell ref="B34:E34"/>
     <mergeCell ref="A2:A3"/>
@@ -2305,45 +2338,13 @@
     <mergeCell ref="E26:E27"/>
     <mergeCell ref="B28:E29"/>
     <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2383,18 +2384,18 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="64" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46" t="s">
+      <c r="B2" s="78"/>
+      <c r="C2" s="78" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="59"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
+      <c r="A3" s="65"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="31" t="s">
@@ -2406,18 +2407,18 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="58" t="s">
+      <c r="A5" s="64" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="40" t="s">
+      <c r="B5" s="80"/>
+      <c r="C5" s="66" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="59"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="41"/>
+      <c r="A6" s="65"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="67"/>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1">
       <c r="A7" s="35" t="s">
@@ -2438,132 +2439,132 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="64" t="s">
         <v>74</v>
       </c>
       <c r="B9" s="27"/>
-      <c r="C9" s="40" t="s">
+      <c r="C9" s="66" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="59"/>
+      <c r="A10" s="65"/>
       <c r="B10" s="22"/>
-      <c r="C10" s="41"/>
+      <c r="C10" s="67"/>
     </row>
     <row r="11" spans="1:3" ht="15" customHeight="1">
-      <c r="A11" s="58" t="s">
+      <c r="A11" s="64" t="s">
         <v>75</v>
       </c>
-      <c r="B11" s="46"/>
-      <c r="C11" s="44" t="s">
+      <c r="B11" s="78"/>
+      <c r="C11" s="74" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="59"/>
-      <c r="B12" s="47"/>
-      <c r="C12" s="45"/>
+      <c r="A12" s="65"/>
+      <c r="B12" s="79"/>
+      <c r="C12" s="75"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="60" t="s">
+      <c r="A13" s="69" t="s">
         <v>76</v>
       </c>
-      <c r="B13" s="42"/>
-      <c r="C13" s="48" t="s">
+      <c r="B13" s="80"/>
+      <c r="C13" s="84" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="60"/>
-      <c r="B14" s="49"/>
-      <c r="C14" s="48"/>
+      <c r="A14" s="69"/>
+      <c r="B14" s="85"/>
+      <c r="C14" s="84"/>
     </row>
     <row r="15" spans="1:3" ht="15" customHeight="1">
-      <c r="A15" s="60" t="s">
+      <c r="A15" s="69" t="s">
         <v>77</v>
       </c>
-      <c r="B15" s="52"/>
-      <c r="C15" s="51" t="s">
+      <c r="B15" s="83"/>
+      <c r="C15" s="82" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="59"/>
-      <c r="B16" s="47"/>
-      <c r="C16" s="45"/>
+      <c r="A16" s="65"/>
+      <c r="B16" s="79"/>
+      <c r="C16" s="75"/>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1">
-      <c r="A17" s="58" t="s">
+      <c r="A17" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="42"/>
-      <c r="C17" s="40" t="s">
+      <c r="B17" s="80"/>
+      <c r="C17" s="66" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="59"/>
-      <c r="B18" s="43"/>
-      <c r="C18" s="41"/>
+      <c r="A18" s="65"/>
+      <c r="B18" s="81"/>
+      <c r="C18" s="67"/>
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1">
-      <c r="A19" s="58"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="44"/>
+      <c r="A19" s="64"/>
+      <c r="B19" s="78"/>
+      <c r="C19" s="74"/>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="59"/>
-      <c r="B20" s="47"/>
-      <c r="C20" s="45"/>
+      <c r="A20" s="65"/>
+      <c r="B20" s="79"/>
+      <c r="C20" s="75"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="58"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="42"/>
+      <c r="A21" s="64"/>
+      <c r="B21" s="80"/>
+      <c r="C21" s="80"/>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="59"/>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
+      <c r="A22" s="65"/>
+      <c r="B22" s="81"/>
+      <c r="C22" s="81"/>
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1">
-      <c r="A23" s="58"/>
-      <c r="B23" s="53"/>
-      <c r="C23" s="53"/>
+      <c r="A23" s="64"/>
+      <c r="B23" s="72"/>
+      <c r="C23" s="72"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="59"/>
-      <c r="B24" s="54"/>
-      <c r="C24" s="54"/>
+      <c r="A24" s="65"/>
+      <c r="B24" s="73"/>
+      <c r="C24" s="73"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="58"/>
+      <c r="A25" s="64"/>
       <c r="B25"/>
       <c r="C25"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="59"/>
+      <c r="A26" s="65"/>
       <c r="B26"/>
       <c r="C26"/>
     </row>
     <row r="27" spans="1:3" ht="15" customHeight="1">
-      <c r="A27" s="58"/>
-      <c r="B27" s="53"/>
-      <c r="C27" s="53"/>
+      <c r="A27" s="64"/>
+      <c r="B27" s="72"/>
+      <c r="C27" s="72"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="59"/>
-      <c r="B28" s="54"/>
-      <c r="C28" s="54"/>
+      <c r="A28" s="65"/>
+      <c r="B28" s="73"/>
+      <c r="C28" s="73"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="58"/>
+      <c r="A29" s="64"/>
       <c r="B29" s="33"/>
       <c r="C29" s="33"/>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="59"/>
+      <c r="A30" s="65"/>
       <c r="B30" s="34"/>
       <c r="C30" s="34"/>
     </row>
@@ -2574,40 +2575,40 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="C23:C24"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="A29:A30"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>